<commit_message>
updated diary, added images, added study results
</commit_message>
<xml_diff>
--- a/ResearchDiary/Questionnaires/sus_evaluate_template.xlsx
+++ b/ResearchDiary/Questionnaires/sus_evaluate_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmaer\Documents\FH\Projects\MasterArbeit\mmt-masterarbeit-david-maerzendorfer\ResearchDiary\Questionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26149882-7209-44BE-B856-F9E4E3069387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505CC4B1-DD7B-4882-AA9A-D30522F51EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="711" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="711" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Completion_Simple" sheetId="12" state="hidden" r:id="rId1"/>
@@ -24,11 +24,14 @@
     <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">SUS_Hover!$Z$12</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">SUS_Hover!$Z$12</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">SUS_Drone!$V$7:$V$18</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">SUS_Hover!$V$7:$V$18</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">SUS_Drone!$V$7:$V$18</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">SUS_Hover!$V$7:$V$18</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">analysis!$D$12</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">SUS_Drone!$V$7:$V$18</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">SUS_Hover!$V$7:$V$18</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">SUS_Drone!$V$7:$V$18</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">SUS_Hover!$V$7:$V$18</definedName>
     <definedName name="Checkbox">[1]Words!$F$1</definedName>
     <definedName name="finding">#REF!</definedName>
     <definedName name="MmExcelLinker_D0610640_9725_4A40_A644_79F42034DD5B" localSheetId="2">Pre-[2]Study!$B$4:$B$4</definedName>
@@ -57,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="70">
   <si>
     <t>Task Completion Effectiveness</t>
   </si>
@@ -421,6 +424,12 @@
   </si>
   <si>
     <t>avg</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>https://measuringu.com/interpret-sus-score/</t>
   </si>
 </sst>
 </file>
@@ -791,6 +800,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -799,9 +811,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2627,12 +2636,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2640,7 +2649,7 @@
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
         <cx:txData>
-          <cx:v>SUS Result</cx:v>
+          <cx:v>SUS Scores for Drone and Hover Camera</cx:v>
         </cx:txData>
       </cx:tx>
       <cx:txPr>
@@ -2660,7 +2669,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>SUS Result</a:t>
+            <a:t>SUS Scores for Drone and Hover Camera</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
@@ -2670,9 +2679,16 @@
         <cx:series layoutId="boxWhisker" uniqueId="{7006A5CA-4D0A-4A4B-ADEE-8489196C325F}">
           <cx:tx>
             <cx:txData>
-              <cx:v>Drone</cx:v>
+              <cx:v>Hover Camera</cx:v>
             </cx:txData>
           </cx:tx>
+          <cx:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
           <cx:dataId val="0"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
@@ -2682,25 +2698,65 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000001-440F-4873-B63B-7B48B26598E1}">
           <cx:tx>
             <cx:txData>
-              <cx:v>Hover</cx:v>
+              <cx:v>Drone Camera</cx:v>
             </cx:txData>
           </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
           <cx:dataId val="1"/>
           <cx:layoutPr>
+            <cx:visibility nonoutliers="0"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
       </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="1"/>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="0.439999998"/>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>SUS Score</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                </a:rPr>
+                <a:t>SUS Score</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
     </cx:plotArea>
+    <cx:legend pos="r" align="ctr" overlay="0"/>
   </cx:chart>
 </cx:chartSpace>
 </file>
@@ -3352,8 +3408,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2644775" y="1485900"/>
-              <a:ext cx="4572000" cy="2740025"/>
+              <a:off x="2644775" y="1482725"/>
+              <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3381,6 +3437,50 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>45563</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>140584</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A07451F-B993-B536-8375-55BFB548F2CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8534400" y="1746250"/>
+          <a:ext cx="7973538" cy="6335009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3721,28 +3821,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="A1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="12" t="s">
@@ -4815,10 +4915,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="41"/>
     </row>
     <row r="3" spans="1:2" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
@@ -4928,7 +5028,7 @@
   <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView topLeftCell="J4" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5662,7 +5762,7 @@
       <c r="A14" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="41">
+      <c r="B14" s="38">
         <v>3</v>
       </c>
       <c r="C14" s="28">
@@ -5744,7 +5844,7 @@
       <c r="A15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="41">
+      <c r="B15" s="38">
         <v>2</v>
       </c>
       <c r="C15" s="28">
@@ -5826,7 +5926,7 @@
       <c r="A16" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="41">
+      <c r="B16" s="38">
         <v>3</v>
       </c>
       <c r="C16" s="28">
@@ -5908,7 +6008,7 @@
       <c r="A17" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="41">
+      <c r="B17" s="38">
         <v>2</v>
       </c>
       <c r="C17" s="28">
@@ -5979,7 +6079,7 @@
         <v>1</v>
       </c>
       <c r="V17" s="29">
-        <f t="shared" ref="V17:V18" si="21">SUM(C17+E17+G17+I17+K17+M17+O17+Q17+S17+U17)*2.5</f>
+        <f t="shared" ref="V17" si="21">SUM(C17+E17+G17+I17+K17+M17+O17+Q17+S17+U17)*2.5</f>
         <v>35</v>
       </c>
       <c r="W17" t="s">
@@ -5990,7 +6090,7 @@
       <c r="A18" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="41">
+      <c r="B18" s="38">
         <v>4</v>
       </c>
       <c r="C18" s="28">
@@ -6075,6 +6175,15 @@
       <c r="V20" s="24">
         <f>AVERAGE(V7:V18)</f>
         <v>57.916666666666664</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U21" t="s">
+        <v>68</v>
+      </c>
+      <c r="V21">
+        <f>STDEV(V7:V18)</f>
+        <v>18.611864902569945</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
@@ -6142,8 +6251,8 @@
   </sheetPr>
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6877,7 +6986,7 @@
       <c r="A14" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="41">
+      <c r="B14" s="38">
         <v>2</v>
       </c>
       <c r="C14" s="28">
@@ -6959,7 +7068,7 @@
       <c r="A15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="41">
+      <c r="B15" s="38">
         <v>2</v>
       </c>
       <c r="C15" s="28">
@@ -7041,7 +7150,7 @@
       <c r="A16" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="41">
+      <c r="B16" s="38">
         <v>4</v>
       </c>
       <c r="C16" s="28">
@@ -7123,7 +7232,7 @@
       <c r="A17" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="41">
+      <c r="B17" s="38">
         <v>4</v>
       </c>
       <c r="C17" s="28">
@@ -7205,7 +7314,7 @@
       <c r="A18" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="41">
+      <c r="B18" s="38">
         <v>5</v>
       </c>
       <c r="C18" s="28">
@@ -7313,6 +7422,15 @@
         <v>73.75</v>
       </c>
     </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U21" t="s">
+        <v>68</v>
+      </c>
+      <c r="V21">
+        <f>STDEV(V7:V18)</f>
+        <v>15.392589716542769</v>
+      </c>
+    </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B22" s="25"/>
       <c r="C22" s="23" t="s">
@@ -7376,14 +7494,20 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="O54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="54" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>